<commit_message>
Bug Fixing Fitur Import Excel
</commit_message>
<xml_diff>
--- a/admin/assets/data_jadwal.xlsx
+++ b/admin/assets/data_jadwal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\smart_door_h6-1\admin\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\smart_door_h6\admin\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02A0C49-5F6A-4415-8B26-601A00A609C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4094959-907D-4169-8A21-D51D6C1EE615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3687CE95-D1C8-436C-A4DC-0FF04842466F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
   <si>
     <t>07.00</t>
   </si>
@@ -64,12 +64,33 @@
   </si>
   <si>
     <t>Ruang Kelas</t>
+  </si>
+  <si>
+    <t>id_jadwal</t>
+  </si>
+  <si>
+    <t>id_mhs</t>
+  </si>
+  <si>
+    <t>tanggal</t>
+  </si>
+  <si>
+    <t>jam_masuk</t>
+  </si>
+  <si>
+    <t>jam_keluar</t>
+  </si>
+  <si>
+    <t>ruangan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +128,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,9 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB709443-8B61-4EEF-B264-04C6247AB2C9}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -435,160 +458,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>9</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>45096</v>
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45096</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
-        <v>45097</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45097</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
-        <v>45098</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>45099</v>
+        <v>45098</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>45100</v>
+        <v>45099</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>45103</v>
+        <v>45100</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>45104</v>
+        <v>45103</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>45105</v>
+        <v>45104</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -596,39 +619,39 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>45106</v>
+        <v>45105</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>45107</v>
+        <v>45106</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -636,106 +659,127 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
-        <v>45110</v>
+        <v>45107</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
-        <v>45111</v>
+        <v>45110</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1">
-        <v>45112</v>
+        <v>45111</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
-        <v>45113</v>
+        <v>45112</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>23</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>45114</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>6</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>